<commit_message>
Fix loading transparent fill
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/TransparentBackgroundFill/TransparentBackgroundFill.xlsx
+++ b/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/TransparentBackgroundFill/TransparentBackgroundFill.xlsx
@@ -89,12 +89,6 @@
       <x:font>
         <x:color theme="1"/>
       </x:font>
-      <x:fill>
-        <x:patternFill patternType="solid">
-          <x:fgColor auto="1"/>
-          <x:bgColor theme="1"/>
-        </x:patternFill>
-      </x:fill>
     </x:dxf>
   </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>

</xml_diff>